<commit_message>
update to most recent
</commit_message>
<xml_diff>
--- a/Λίστα γραφείων καθηγητών.xlsx
+++ b/Λίστα γραφείων καθηγητών.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\pvyro\Documents\Projects\PaspMapsApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F74C9D13-19B8-46EF-907E-DDCC52F67E67}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E051FD37-23C0-45DF-84AE-D4747C34D054}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{AC6D25AB-5769-4605-A116-69C7152FFB08}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ProfOffices" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>ID</t>
   </si>
@@ -47,15 +47,47 @@
   <si>
     <t>Τηλέφωνο</t>
   </si>
+  <si>
+    <t>ΤΕΣΤ1</t>
+  </si>
+  <si>
+    <t>ΤΕΣΤ2</t>
+  </si>
+  <si>
+    <t>ΤΣΕΤ1</t>
+  </si>
+  <si>
+    <t>asd@asd.com</t>
+  </si>
+  <si>
+    <t>Β.098</t>
+  </si>
+  <si>
+    <t>ΤΣΕΤ2</t>
+  </si>
+  <si>
+    <t>aqweqe@vdfjvio.gr</t>
+  </si>
+  <si>
+    <t>Α.104</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -78,13 +110,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -399,9 +434,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98B97EBD-64F6-463E-A99D-9FA7B1F68D55}">
   <dimension ref="A1:G270"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -440,11 +473,47 @@
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>2154002488</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>2541896302</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -2055,6 +2124,10 @@
       <formula1>"1, 2, 3, 4"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{8283068F-FB41-4F9F-A6EF-5A171C024499}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{8977E024-7AB0-46F3-AEBF-8EC885AAC52E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>